<commit_message>
add gitignore, add S1
</commit_message>
<xml_diff>
--- a/Analyses/CAMspiracy/t2_CAMs/outputs/questionnaireCAMs.xlsx
+++ b/Analyses/CAMspiracy/t2_CAMs/outputs/questionnaireCAMs.xlsx
@@ -2425,7 +2425,7 @@
         <v>0.6723484848484849</v>
       </c>
       <c r="BE3" t="n">
-        <v>0.7039631414544355</v>
+        <v>0.7039631414544361</v>
       </c>
       <c r="BF3" t="n">
         <v>3.5789473684210527</v>
@@ -2909,7 +2909,7 @@
         <v>0.6742424242424242</v>
       </c>
       <c r="BE5" t="n">
-        <v>0.7256314504280088</v>
+        <v>0.7256314504280085</v>
       </c>
       <c r="BF5" t="n">
         <v>4.517241379310345</v>
@@ -3393,7 +3393,7 @@
         <v>0.8699494949494949</v>
       </c>
       <c r="BE7" t="n">
-        <v>0.7730948816876565</v>
+        <v>0.7730948816876567</v>
       </c>
       <c r="BF7" t="n">
         <v>3.391304347826087</v>
@@ -3635,7 +3635,7 @@
         <v>0.7950413223140496</v>
       </c>
       <c r="BE8" t="n">
-        <v>0.6992949937059293</v>
+        <v>0.6992949937059292</v>
       </c>
       <c r="BF8" t="n">
         <v>3.6</v>
@@ -3877,7 +3877,7 @@
         <v>0.40067340067340057</v>
       </c>
       <c r="BE9" t="n">
-        <v>0.5001923783242049</v>
+        <v>0.500192378324205</v>
       </c>
       <c r="BF9" t="n">
         <v>3.017543859649123</v>
@@ -4119,7 +4119,7 @@
         <v>0.4940828402366864</v>
       </c>
       <c r="BE10" t="n">
-        <v>0.6661966366553171</v>
+        <v>0.6661966366553168</v>
       </c>
       <c r="BF10" t="n">
         <v>6.016949152542373</v>
@@ -4361,7 +4361,7 @@
         <v>0.4911616161616162</v>
       </c>
       <c r="BE11" t="n">
-        <v>0.6687610599583357</v>
+        <v>0.6687610599583359</v>
       </c>
       <c r="BF11" t="n">
         <v>6.057142857142857</v>
@@ -4603,7 +4603,7 @@
         <v>0.9488636363636364</v>
       </c>
       <c r="BE12" t="n">
-        <v>0.7643437522066275</v>
+        <v>0.7643437522066274</v>
       </c>
       <c r="BF12" t="n">
         <v>2.3902439024390243</v>
@@ -5087,7 +5087,7 @@
         <v>0.5256410256410257</v>
       </c>
       <c r="BE14" t="n">
-        <v>0.6445011396907578</v>
+        <v>0.6445011396907581</v>
       </c>
       <c r="BF14" t="n">
         <v>4.5</v>
@@ -5329,7 +5329,7 @@
         <v>1.0</v>
       </c>
       <c r="BE15" t="n">
-        <v>0.7759907622602042</v>
+        <v>0.7759907622602039</v>
       </c>
       <c r="BF15" t="n">
         <v>1.625</v>
@@ -5813,7 +5813,7 @@
         <v>0.8005050505050505</v>
       </c>
       <c r="BE17" t="n">
-        <v>0.7094200825169513</v>
+        <v>0.7094200825169515</v>
       </c>
       <c r="BF17" t="n">
         <v>3.425925925925926</v>
@@ -6055,7 +6055,7 @@
         <v>0.5943458251150558</v>
       </c>
       <c r="BE18" t="n">
-        <v>0.6384209554272582</v>
+        <v>0.6384209554272583</v>
       </c>
       <c r="BF18" t="n">
         <v>5.568181818181818</v>
@@ -6297,7 +6297,7 @@
         <v>0.4659090909090909</v>
       </c>
       <c r="BE19" t="n">
-        <v>0.6800727431914517</v>
+        <v>0.680072743191452</v>
       </c>
       <c r="BF19" t="n">
         <v>1.641025641025641</v>
@@ -6539,7 +6539,7 @@
         <v>0.18543956043956045</v>
       </c>
       <c r="BE20" t="n">
-        <v>0.5836291076644482</v>
+        <v>0.5836291076644474</v>
       </c>
       <c r="BF20" t="n">
         <v>5.4520547945205475</v>
@@ -6781,7 +6781,7 @@
         <v>0.6656200941915228</v>
       </c>
       <c r="BE21" t="n">
-        <v>0.7456299505271807</v>
+        <v>0.7456299505271813</v>
       </c>
       <c r="BF21" t="n">
         <v>5.257142857142857</v>
@@ -7023,7 +7023,7 @@
         <v>0.8648915187376726</v>
       </c>
       <c r="BE22" t="n">
-        <v>0.7802593038528179</v>
+        <v>0.7802593038528182</v>
       </c>
       <c r="BF22" t="n">
         <v>1.7222222222222223</v>
@@ -7265,7 +7265,7 @@
         <v>0.5482731554160125</v>
       </c>
       <c r="BE23" t="n">
-        <v>0.6305888847153072</v>
+        <v>0.6305888847153062</v>
       </c>
       <c r="BF23" t="n">
         <v>3.0833333333333335</v>
@@ -7749,7 +7749,7 @@
         <v>0.44938973063973064</v>
       </c>
       <c r="BE25" t="n">
-        <v>0.5604292923717348</v>
+        <v>0.5604292923717347</v>
       </c>
       <c r="BF25" t="n">
         <v>2.1327433628318584</v>
@@ -8233,7 +8233,7 @@
         <v>0.9818181818181818</v>
       </c>
       <c r="BE27" t="n">
-        <v>0.7561930600795045</v>
+        <v>0.7561930600795044</v>
       </c>
       <c r="BF27" t="n">
         <v>2.6666666666666665</v>
@@ -8959,7 +8959,7 @@
         <v>0.6981946624803768</v>
       </c>
       <c r="BE30" t="n">
-        <v>0.7545868038477971</v>
+        <v>0.7545868038477972</v>
       </c>
       <c r="BF30" t="n">
         <v>2.4310344827586206</v>
@@ -9201,7 +9201,7 @@
         <v>0.39641003460207613</v>
       </c>
       <c r="BE31" t="n">
-        <v>0.6416182230273741</v>
+        <v>0.6416182230273744</v>
       </c>
       <c r="BF31" t="n">
         <v>5.7894736842105265</v>
@@ -9685,7 +9685,7 @@
         <v>0.3869165023011177</v>
       </c>
       <c r="BE33" t="n">
-        <v>0.5535908241110464</v>
+        <v>0.5535908241110465</v>
       </c>
       <c r="BF33" t="n">
         <v>5.504504504504505</v>
@@ -10411,7 +10411,7 @@
         <v>0.3194662480376766</v>
       </c>
       <c r="BE36" t="n">
-        <v>0.6561121091631203</v>
+        <v>0.6561121091631205</v>
       </c>
       <c r="BF36" t="n">
         <v>4.222222222222222</v>
@@ -10895,7 +10895,7 @@
         <v>0.7159090909090909</v>
       </c>
       <c r="BE38" t="n">
-        <v>0.6948826958819585</v>
+        <v>0.6948826958819588</v>
       </c>
       <c r="BF38" t="n">
         <v>6.519230769230769</v>
@@ -11137,7 +11137,7 @@
         <v>0.6351084812623274</v>
       </c>
       <c r="BE39" t="n">
-        <v>0.773349315383926</v>
+        <v>0.7733493153839263</v>
       </c>
       <c r="BF39" t="n">
         <v>1.3333333333333333</v>
@@ -11377,7 +11377,7 @@
         <v>0.7746539792387545</v>
       </c>
       <c r="BE40" t="n">
-        <v>0.744804247089552</v>
+        <v>0.7448042470895523</v>
       </c>
       <c r="BF40" t="n">
         <v>4.2272727272727275</v>
@@ -12103,7 +12103,7 @@
         <v>0.6300505050505051</v>
       </c>
       <c r="BE43" t="n">
-        <v>0.6814509521019754</v>
+        <v>0.6814509521019757</v>
       </c>
       <c r="BF43" t="n">
         <v>1.4838709677419355</v>
@@ -12829,7 +12829,7 @@
         <v>0.31786948853615515</v>
       </c>
       <c r="BE46" t="n">
-        <v>0.6109976549649961</v>
+        <v>0.6109976549649963</v>
       </c>
       <c r="BF46" t="n">
         <v>2.888</v>
@@ -13071,7 +13071,7 @@
         <v>0.8598484848484849</v>
       </c>
       <c r="BE47" t="n">
-        <v>0.7117226763030792</v>
+        <v>0.7117226763030788</v>
       </c>
       <c r="BF47" t="n">
         <v>4.1</v>
@@ -14039,7 +14039,7 @@
         <v>0.5795454545454546</v>
       </c>
       <c r="BE51" t="n">
-        <v>0.5876751203535703</v>
+        <v>0.5876751203535707</v>
       </c>
       <c r="BF51" t="n">
         <v>1.52</v>
@@ -14523,7 +14523,7 @@
         <v>0.8181818181818182</v>
       </c>
       <c r="BE53" t="n">
-        <v>0.6991548881373778</v>
+        <v>0.6991548881373773</v>
       </c>
       <c r="BF53" t="n">
         <v>3.4375</v>
@@ -14765,7 +14765,7 @@
         <v>1.0</v>
       </c>
       <c r="BE54" t="n">
-        <v>0.7759907622602039</v>
+        <v>0.7759907622602042</v>
       </c>
       <c r="BF54" t="n">
         <v>4.212765957446808</v>
@@ -15249,7 +15249,7 @@
         <v>0.2632996632996633</v>
       </c>
       <c r="BE56" t="n">
-        <v>0.5579632877250359</v>
+        <v>0.5579632877250356</v>
       </c>
       <c r="BF56" t="n">
         <v>4.096774193548387</v>
@@ -15491,7 +15491,7 @@
         <v>1.0</v>
       </c>
       <c r="BE57" t="n">
-        <v>0.76833752096446</v>
+        <v>0.7683375209644601</v>
       </c>
       <c r="BF57" t="n">
         <v>2.1379310344827585</v>
@@ -15733,7 +15733,7 @@
         <v>0.7001972386587771</v>
       </c>
       <c r="BE58" t="n">
-        <v>0.721472565065563</v>
+        <v>0.7214725650655627</v>
       </c>
       <c r="BF58" t="n">
         <v>4.585365853658536</v>
@@ -15975,7 +15975,7 @@
         <v>0.740484429065744</v>
       </c>
       <c r="BE59" t="n">
-        <v>0.7467269103335876</v>
+        <v>0.7467269103335875</v>
       </c>
       <c r="BF59" t="n">
         <v>2.727272727272727</v>
@@ -16459,7 +16459,7 @@
         <v>0.5250544662309368</v>
       </c>
       <c r="BE61" t="n">
-        <v>0.609623541202747</v>
+        <v>0.6096235412027468</v>
       </c>
       <c r="BF61" t="n">
         <v>3.408333333333333</v>
@@ -16701,7 +16701,7 @@
         <v>0.4696969696969697</v>
       </c>
       <c r="BE62" t="n">
-        <v>0.6303361469402873</v>
+        <v>0.6303361469402874</v>
       </c>
       <c r="BF62" t="n">
         <v>2.65</v>
@@ -16943,7 +16943,7 @@
         <v>0.9381313131313131</v>
       </c>
       <c r="BE63" t="n">
-        <v>0.7419796269483416</v>
+        <v>0.7419796269483414</v>
       </c>
       <c r="BF63" t="n">
         <v>1.6875</v>
@@ -17427,7 +17427,7 @@
         <v>0.3586456278763971</v>
       </c>
       <c r="BE65" t="n">
-        <v>0.6591804531074176</v>
+        <v>0.6591804531074175</v>
       </c>
       <c r="BF65" t="n">
         <v>5.34</v>
@@ -17669,7 +17669,7 @@
         <v>0.6883830455259027</v>
       </c>
       <c r="BE66" t="n">
-        <v>0.7670059672747954</v>
+        <v>0.7670059672747958</v>
       </c>
       <c r="BF66" t="n">
         <v>4.764705882352941</v>
@@ -18153,7 +18153,7 @@
         <v>0.6301775147928994</v>
       </c>
       <c r="BE68" t="n">
-        <v>0.6487310688403939</v>
+        <v>0.6487310688403934</v>
       </c>
       <c r="BF68" t="n">
         <v>2.967741935483871</v>
@@ -18637,7 +18637,7 @@
         <v>0.4751683501683501</v>
       </c>
       <c r="BE70" t="n">
-        <v>0.6995900777392827</v>
+        <v>0.699590077739283</v>
       </c>
       <c r="BF70" t="n">
         <v>1.8157894736842106</v>
@@ -19121,7 +19121,7 @@
         <v>0.1671085858585859</v>
       </c>
       <c r="BE72" t="n">
-        <v>0.41501885289083923</v>
+        <v>0.4150188528908394</v>
       </c>
       <c r="BF72" t="n">
         <v>4.8977272727272725</v>
@@ -19361,7 +19361,7 @@
         <v>0.40622895622895616</v>
       </c>
       <c r="BE73" t="n">
-        <v>0.5890297335340974</v>
+        <v>0.5890297335340976</v>
       </c>
       <c r="BF73" t="n">
         <v>6.423076923076923</v>
@@ -19603,7 +19603,7 @@
         <v>0.5128205128205128</v>
       </c>
       <c r="BE74" t="n">
-        <v>0.6541075676695761</v>
+        <v>0.6541075676695763</v>
       </c>
       <c r="BF74" t="n">
         <v>5.931818181818182</v>
@@ -20087,7 +20087,7 @@
         <v>0.6856060606060606</v>
       </c>
       <c r="BE76" t="n">
-        <v>0.6903631718354526</v>
+        <v>0.6903631718354523</v>
       </c>
       <c r="BF76" t="n">
         <v>1.72</v>
@@ -20329,7 +20329,7 @@
         <v>0.39730639730639733</v>
       </c>
       <c r="BE77" t="n">
-        <v>0.6646145954904613</v>
+        <v>0.6646145954904612</v>
       </c>
       <c r="BF77" t="n">
         <v>3.475</v>
@@ -20813,7 +20813,7 @@
         <v>0.8421717171717171</v>
       </c>
       <c r="BE79" t="n">
-        <v>0.7633270405226223</v>
+        <v>0.7633270405226221</v>
       </c>
       <c r="BF79" t="n">
         <v>3.48</v>
@@ -21045,7 +21045,7 @@
         <v>0.5851239669421487</v>
       </c>
       <c r="BE80" t="n">
-        <v>0.6929632483024005</v>
+        <v>0.6929632483024009</v>
       </c>
       <c r="BF80" t="n">
         <v>1.7272727272727273</v>
@@ -21287,7 +21287,7 @@
         <v>0.7563131313131313</v>
       </c>
       <c r="BE81" t="n">
-        <v>0.6818432807724645</v>
+        <v>0.6818432807724643</v>
       </c>
       <c r="BF81" t="n">
         <v>1.84375</v>
@@ -21771,7 +21771,7 @@
         <v>1.0</v>
       </c>
       <c r="BE83" t="n">
-        <v>0.7759907622602042</v>
+        <v>0.775990762260204</v>
       </c>
       <c r="BF83" t="n">
         <v>1.7446808510638299</v>
@@ -22247,7 +22247,7 @@
         <v>0.5661718750000001</v>
       </c>
       <c r="BE85" t="n">
-        <v>0.6724618248782624</v>
+        <v>0.6724618248782626</v>
       </c>
       <c r="BF85" t="n">
         <v>2.6161137440758293</v>
@@ -22489,7 +22489,7 @@
         <v>0.6891679748822606</v>
       </c>
       <c r="BE86" t="n">
-        <v>0.691973782751383</v>
+        <v>0.6919737827513829</v>
       </c>
       <c r="BF86" t="n">
         <v>1.375</v>
@@ -22973,7 +22973,7 @@
         <v>0.18550084175084178</v>
       </c>
       <c r="BE88" t="n">
-        <v>0.48924340278679357</v>
+        <v>0.48924340278679374</v>
       </c>
       <c r="BF88" t="n">
         <v>7.4</v>
@@ -23455,7 +23455,7 @@
         <v>0.7060439560439561</v>
       </c>
       <c r="BE90" t="n">
-        <v>0.6669611518351825</v>
+        <v>0.6669611518351821</v>
       </c>
       <c r="BF90" t="n">
         <v>2.127659574468085</v>
@@ -23929,7 +23929,7 @@
         <v>0.2819834710743802</v>
       </c>
       <c r="BE92" t="n">
-        <v>0.328601761666982</v>
+        <v>0.32860176166698185</v>
       </c>
       <c r="BF92" t="n">
         <v>3.2222222222222223</v>
@@ -24171,7 +24171,7 @@
         <v>0.4972643097643097</v>
       </c>
       <c r="BE93" t="n">
-        <v>0.6061860976384703</v>
+        <v>0.6061860976384709</v>
       </c>
       <c r="BF93" t="n">
         <v>6.856060606060606</v>
@@ -24413,7 +24413,7 @@
         <v>0.5464856902356902</v>
       </c>
       <c r="BE94" t="n">
-        <v>0.6728497817027042</v>
+        <v>0.672849781702704</v>
       </c>
       <c r="BF94" t="n">
         <v>4.3076923076923075</v>
@@ -24655,7 +24655,7 @@
         <v>0.5355371900826447</v>
       </c>
       <c r="BE95" t="n">
-        <v>0.6794615015976849</v>
+        <v>0.6794615015976846</v>
       </c>
       <c r="BF95" t="n">
         <v>3.696969696969697</v>
@@ -24897,7 +24897,7 @@
         <v>0.6382575757575758</v>
       </c>
       <c r="BE96" t="n">
-        <v>0.7514790618967374</v>
+        <v>0.7514790618967372</v>
       </c>
       <c r="BF96" t="n">
         <v>2.227272727272727</v>
@@ -25139,7 +25139,7 @@
         <v>0.8358585858585859</v>
       </c>
       <c r="BE97" t="n">
-        <v>0.7243148930851245</v>
+        <v>0.7243148930851243</v>
       </c>
       <c r="BF97" t="n">
         <v>2.27027027027027</v>
@@ -25381,7 +25381,7 @@
         <v>0.7291666666666666</v>
       </c>
       <c r="BE98" t="n">
-        <v>0.7281974999558514</v>
+        <v>0.7281974999558515</v>
       </c>
       <c r="BF98" t="n">
         <v>2.5238095238095237</v>
@@ -26833,7 +26833,7 @@
         <v>0.23758417508417512</v>
       </c>
       <c r="BE104" t="n">
-        <v>0.5248565426737831</v>
+        <v>0.5248565426737829</v>
       </c>
       <c r="BF104" t="n">
         <v>5.855555555555555</v>
@@ -27075,7 +27075,7 @@
         <v>0.5140495867768595</v>
       </c>
       <c r="BE105" t="n">
-        <v>0.5035429159959741</v>
+        <v>0.5035429159959743</v>
       </c>
       <c r="BF105" t="n">
         <v>4.011627906976744</v>
@@ -27317,7 +27317,7 @@
         <v>0.5088383838383839</v>
       </c>
       <c r="BE106" t="n">
-        <v>0.5298498999513523</v>
+        <v>0.5298498999513526</v>
       </c>
       <c r="BF106" t="n">
         <v>2.2045454545454546</v>
@@ -27559,7 +27559,7 @@
         <v>0.5801652892561984</v>
       </c>
       <c r="BE107" t="n">
-        <v>0.5996258034517246</v>
+        <v>0.5996258034517238</v>
       </c>
       <c r="BF107" t="n">
         <v>1.588235294117647</v>
@@ -27801,7 +27801,7 @@
         <v>0.577020202020202</v>
       </c>
       <c r="BE108" t="n">
-        <v>0.5919173910257378</v>
+        <v>0.591917391025738</v>
       </c>
       <c r="BF108" t="n">
         <v>2.7625</v>
@@ -28043,7 +28043,7 @@
         <v>0.509469696969697</v>
       </c>
       <c r="BE109" t="n">
-        <v>0.6856155533238779</v>
+        <v>0.6856155533238778</v>
       </c>
       <c r="BF109" t="n">
         <v>2.8</v>
@@ -28285,7 +28285,7 @@
         <v>1.0</v>
       </c>
       <c r="BE110" t="n">
-        <v>0.7759907622602039</v>
+        <v>0.7759907622602042</v>
       </c>
       <c r="BF110" t="n">
         <v>1.6923076923076923</v>
@@ -28527,7 +28527,7 @@
         <v>0.6475168350168351</v>
       </c>
       <c r="BE111" t="n">
-        <v>0.6949192071523786</v>
+        <v>0.6949192071523782</v>
       </c>
       <c r="BF111" t="n">
         <v>2.3043478260869565</v>
@@ -28769,7 +28769,7 @@
         <v>0.6081649831649831</v>
       </c>
       <c r="BE112" t="n">
-        <v>0.5885273831521239</v>
+        <v>0.5885273831521244</v>
       </c>
       <c r="BF112" t="n">
         <v>5.152941176470589</v>
@@ -29253,7 +29253,7 @@
         <v>0.7933884297520661</v>
       </c>
       <c r="BE114" t="n">
-        <v>0.7387592154231896</v>
+        <v>0.7387592154231895</v>
       </c>
       <c r="BF114" t="n">
         <v>1.72</v>
@@ -29737,7 +29737,7 @@
         <v>0.6760330578512397</v>
       </c>
       <c r="BE116" t="n">
-        <v>0.6817290787845065</v>
+        <v>0.6817290787845061</v>
       </c>
       <c r="BF116" t="n">
         <v>3.4516129032258065</v>
@@ -29929,7 +29929,7 @@
         <v>0.44297520661157025</v>
       </c>
       <c r="BE117" t="n">
-        <v>0.6531555214579817</v>
+        <v>0.6531555214579816</v>
       </c>
       <c r="BF117" t="n">
         <v>2.40625</v>
@@ -30413,7 +30413,7 @@
         <v>0.5997474747474747</v>
       </c>
       <c r="BE119" t="n">
-        <v>0.640203549287784</v>
+        <v>0.6402035492877843</v>
       </c>
       <c r="BF119" t="n">
         <v>4.785714285714286</v>
@@ -30655,7 +30655,7 @@
         <v>0.6483516483516484</v>
       </c>
       <c r="BE120" t="n">
-        <v>0.6438228895554107</v>
+        <v>0.6438228895554112</v>
       </c>
       <c r="BF120" t="n">
         <v>3.9056603773584904</v>
@@ -31381,7 +31381,7 @@
         <v>0.5950413223140496</v>
       </c>
       <c r="BE123" t="n">
-        <v>0.577768692715763</v>
+        <v>0.5777686927157629</v>
       </c>
       <c r="BF123" t="n">
         <v>1.4285714285714286</v>
@@ -31621,7 +31621,7 @@
         <v>0.32386363636363635</v>
       </c>
       <c r="BE124" t="n">
-        <v>0.5757134300352923</v>
+        <v>0.575713430035292</v>
       </c>
       <c r="BF124" t="n">
         <v>6.988095238095238</v>
@@ -32105,7 +32105,7 @@
         <v>0.4577020202020202</v>
       </c>
       <c r="BE126" t="n">
-        <v>0.6448484920261272</v>
+        <v>0.6448484920261274</v>
       </c>
       <c r="BF126" t="n">
         <v>2.925925925925926</v>
@@ -32347,7 +32347,7 @@
         <v>0.6313131313131313</v>
       </c>
       <c r="BE127" t="n">
-        <v>0.6894245115331001</v>
+        <v>0.6894245115331002</v>
       </c>
       <c r="BF127" t="n">
         <v>2.2857142857142856</v>
@@ -32589,7 +32589,7 @@
         <v>0.6808021038790268</v>
       </c>
       <c r="BE128" t="n">
-        <v>0.660262705768093</v>
+        <v>0.6602627057680931</v>
       </c>
       <c r="BF128" t="n">
         <v>5.120689655172414</v>
@@ -32831,7 +32831,7 @@
         <v>0.4930555555555556</v>
       </c>
       <c r="BE129" t="n">
-        <v>0.6547605022189076</v>
+        <v>0.6547605022189077</v>
       </c>
       <c r="BF129" t="n">
         <v>1.56</v>
@@ -33073,7 +33073,7 @@
         <v>0.1905982905982906</v>
       </c>
       <c r="BE130" t="n">
-        <v>0.5231772525081397</v>
+        <v>0.5231772525081395</v>
       </c>
       <c r="BF130" t="n">
         <v>2.2058823529411766</v>
@@ -33265,7 +33265,7 @@
         <v>0.35374579124579125</v>
       </c>
       <c r="BE131" t="n">
-        <v>0.5153779723093671</v>
+        <v>0.5153779723093672</v>
       </c>
       <c r="BF131" t="n">
         <v>3.076923076923077</v>

</xml_diff>